<commit_message>
added testing and database files to REadme
</commit_message>
<xml_diff>
--- a/media/files/TestResultsMS4.xlsx
+++ b/media/files/TestResultsMS4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C842F1B-7C21-4F60-B7C4-FBEAAF905C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDC716-C96D-49D5-981B-85F2AD543149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-2190" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
   <si>
     <t>Test Case</t>
   </si>
@@ -96,15 +96,9 @@
     <t>Nav Menu Links</t>
   </si>
   <si>
-    <t>EmailJS Works - Email Received with  User Input</t>
-  </si>
-  <si>
     <t>All content is rendered correctly</t>
   </si>
   <si>
-    <t>Email received</t>
-  </si>
-  <si>
     <t>All lead to the correct destination</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>1) Open website 2) Click on the buttons one by one 3) Check they lead to the desired Social Media Platform and that they are opened in a new window.</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Open website 2) Go to the Contact Page 3) Fill the form taking into account the expected type of input in each field (Name -&gt; Text </t>
-  </si>
-  <si>
     <t>Contact forms checks that the input is correct and displays an alert message notifying the visitor that the request was susccesfully submitted.</t>
   </si>
   <si>
@@ -168,18 +159,6 @@
     <t>Profile Page is ok, all buttons work and users data is shown</t>
   </si>
   <si>
-    <t>Show Resources functions display all user resources</t>
-  </si>
-  <si>
-    <t>Hide Resources Hide account Ressources</t>
-  </si>
-  <si>
-    <t>Edit Resources works Properly</t>
-  </si>
-  <si>
-    <t>Resources can be Deleted</t>
-  </si>
-  <si>
     <t>Search Function displays pertinent results</t>
   </si>
   <si>
@@ -201,9 +180,6 @@
     <t>Contact Form Checks Work</t>
   </si>
   <si>
-    <t>Email Received</t>
-  </si>
-  <si>
     <t>All Profile Buttons and Functionalities work properly</t>
   </si>
   <si>
@@ -213,39 +189,6 @@
     <t>Works Properly</t>
   </si>
   <si>
-    <t>Resources are Shown</t>
-  </si>
-  <si>
-    <t>Resources showed</t>
-  </si>
-  <si>
-    <t>Resources get Hid</t>
-  </si>
-  <si>
-    <t>Resources Hid</t>
-  </si>
-  <si>
-    <t>Resources can be edited</t>
-  </si>
-  <si>
-    <t>Resources can be deleted</t>
-  </si>
-  <si>
-    <t>Check that they get displayed after logging in, registering and so on</t>
-  </si>
-  <si>
-    <t>It should be possible to hide all  resource from the user by clicking on the Hide Resources Button.</t>
-  </si>
-  <si>
-    <t>It should be possible to show all  resource from the user by clicking on the Show Resources Button.</t>
-  </si>
-  <si>
-    <t>It should be possible to edit all  resource from the user by clicking on the Edit Resources Button.</t>
-  </si>
-  <si>
-    <t>It should be possible to delete all  resource from the user by clicking on the Delete Resources Button.</t>
-  </si>
-  <si>
     <t>Enter email and password of an accounton the log in page. Then we should get redirected to their profile page</t>
   </si>
   <si>
@@ -312,24 +255,6 @@
     <t>TC022</t>
   </si>
   <si>
-    <t>TC023</t>
-  </si>
-  <si>
-    <t>TC024</t>
-  </si>
-  <si>
-    <t>TC025</t>
-  </si>
-  <si>
-    <t>Toasts Get Displayed Properly</t>
-  </si>
-  <si>
-    <t>Toasts Correctly Displayed</t>
-  </si>
-  <si>
-    <t>They work</t>
-  </si>
-  <si>
     <t xml:space="preserve">Profile Details can be modified. </t>
   </si>
   <si>
@@ -339,15 +264,6 @@
     <t>All ok</t>
   </si>
   <si>
-    <t>Go to Product managemente and add a new product</t>
-  </si>
-  <si>
-    <t>Products Get Added properly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add new Products </t>
-  </si>
-  <si>
     <t>Contact Info - It is possible to send an email to the company through email link</t>
   </si>
   <si>
@@ -366,15 +282,6 @@
     <t>Click on the arrows to switch picture/review</t>
   </si>
   <si>
-    <t>TC026</t>
-  </si>
-  <si>
-    <t>TC027</t>
-  </si>
-  <si>
-    <t>TC028</t>
-  </si>
-  <si>
     <t>It is possible to check out paying using stripe API</t>
   </si>
   <si>
@@ -385,13 +292,34 @@
   </si>
   <si>
     <t>Go to the profile page and check user's orders</t>
+  </si>
+  <si>
+    <t>Admin Product Management - Capable of Adding Products</t>
+  </si>
+  <si>
+    <t>Admin Product Management - Capable of Editing Products</t>
+  </si>
+  <si>
+    <t>Admin Product Management - Capable of Deleting Products</t>
+  </si>
+  <si>
+    <t>Go To Product Management, Select Add New Product, try to submit the form. Check if product was added</t>
+  </si>
+  <si>
+    <t>Go To Product Management, Click on a Product, Edit it and try to submit the form. Check if product was modified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open website 2) Go to the Form Page 3) Fill the form taking into account the expected type of input in each field </t>
+  </si>
+  <si>
+    <t>Go To Product Management, Click on a Product, Click Delete and try to submit the form. Check if product was eliminated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,26 +356,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -469,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -485,26 +393,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2554BD27-039A-455E-B163-8556DA546CCB}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>4</v>
@@ -829,16 +718,16 @@
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -849,16 +738,16 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -869,16 +758,16 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -889,16 +778,16 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -909,16 +798,16 @@
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -926,19 +815,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -946,19 +835,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,19 +855,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -986,19 +875,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1006,19 +895,19 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1026,379 +915,295 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>28</v>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="12" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="13" t="s">
+      <c r="E21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>28</v>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" t="s">
-        <v>28</v>
-      </c>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" t="s">
-        <v>28</v>
-      </c>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" t="s">
-        <v>28</v>
-      </c>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="F32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F35" t="s">
-        <v>28</v>
-      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>